<commit_message>
Atualização tabela de pontuação
</commit_message>
<xml_diff>
--- a/documentos/Backlog Requisitos.xlsx
+++ b/documentos/Backlog Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/henrique_coelho_sptech_school/Documents/SPTECH/Sprint2/sprint2/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F7D1B04D-B3ED-4B34-9640-7573DB81BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EA2BBA8-F2FB-40A0-9BB9-2D9F1DC7F982}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F7D1B04D-B3ED-4B34-9640-7573DB81BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B12569C-190D-42D3-A137-3612296A0CF0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
   <si>
     <t>Requisitos</t>
   </si>
@@ -354,13 +354,22 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t>Pontuação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requisitos do Site </t>
+  </si>
+  <si>
+    <t>Geral</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,8 +409,21 @@
       <name val="Bahnschrift Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Bahnschrift SemiBold"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Bahnschrift SemiBold"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,6 +440,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -609,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -633,6 +661,42 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,56 +718,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,23 +1222,23 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
     </row>
     <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
@@ -1541,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7DA6DA-76F6-4BBF-B420-7F89428DFE23}">
-  <dimension ref="B2:J31"/>
+  <dimension ref="B2:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1553,414 +1608,442 @@
     <col min="3" max="3" width="53.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-    </row>
-    <row r="5" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="L6" s="35"/>
+    </row>
+    <row r="7" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="J7" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-    </row>
-    <row r="9" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+      <c r="D8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="J8" s="39">
+        <f>SUM(F6:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <f>SUM(F22:F31)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="41">
+        <f>SUM(J8:K8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20" t="s">
+      <c r="D10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-    </row>
-    <row r="12" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
+      <c r="D12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
+      <c r="D13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="2:10" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="D15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="2:8" ht="19.05" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:8" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="13" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="27"/>
+      <c r="D22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="29"/>
+      <c r="D23" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="27"/>
+      <c r="D24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="29"/>
+      <c r="D25" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="17"/>
     </row>
     <row r="26" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="27"/>
+      <c r="D26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="29"/>
+      <c r="D27" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="27"/>
+      <c r="D28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="29"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="27"/>
+      <c r="D30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="2:8" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="32"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Backlog de requisitos com os pesos
</commit_message>
<xml_diff>
--- a/documentos/Backlog Requisitos.xlsx
+++ b/documentos/Backlog Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/henrique_coelho_sptech_school/Documents/SPTECH/Sprint2/sprint2/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F7D1B04D-B3ED-4B34-9640-7573DB81BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59F7FA13-E29B-43A5-977E-DBCD1B1FF3E2}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{F7D1B04D-B3ED-4B34-9640-7573DB81BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E07D051-69A4-4F4A-BACB-2288EB9B11AF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="118">
   <si>
     <t>Requisitos</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Criar um código onde será feita a captura de dados do sensor de bloqueio e inclui-los em um gráfico</t>
   </si>
   <si>
-    <t>Requisitos do site</t>
-  </si>
-  <si>
     <t>Sessão Início</t>
   </si>
   <si>
@@ -323,12 +320,6 @@
     <t>Criar e configurar no GitHub</t>
   </si>
   <si>
-    <t>Site institucional</t>
-  </si>
-  <si>
-    <t>Criar um site institucional a partir dos protótipos selecionados</t>
-  </si>
-  <si>
     <t>Sessão Calculadora</t>
   </si>
   <si>
@@ -363,6 +354,39 @@
   </si>
   <si>
     <t>Geral</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código da calculadora </t>
+  </si>
+  <si>
+    <t>Desenvolvimento da lógica e do código da calculadora</t>
+  </si>
+  <si>
+    <t>lógica do Login</t>
+  </si>
+  <si>
+    <t>Validação dos dados inseridos pelo usuário e retornar permissão.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lógica do cadastro </t>
+  </si>
+  <si>
+    <t>Coletar e validar as informações cadastrais e gravar no banco de dados</t>
   </si>
 </sst>
 </file>
@@ -444,7 +468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,7 +698,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -707,33 +731,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -743,6 +740,42 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,51 +783,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1259,23 +1247,23 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
@@ -1633,10 +1621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7DA6DA-76F6-4BBF-B420-7F89428DFE23}">
-  <dimension ref="B2:L31"/>
+  <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,35 +1639,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -1692,16 +1680,16 @@
         <v>2</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>103</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1714,65 +1702,79 @@
       <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="10">
+        <v>13</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="J6" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="41"/>
+      <c r="J6" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="25"/>
+      <c r="L6" s="26"/>
     </row>
     <row r="7" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>68</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="E7" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="11">
+        <v>3</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
       <c r="H7" s="11"/>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>109</v>
+      <c r="K7" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="10">
+        <v>5</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
-      <c r="J8" s="24">
-        <f>SUM(F6:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="25">
-        <f>SUM(F22:F31)</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="26">
+      <c r="J8" s="27">
+        <f>SUM(F8:F16)</f>
+        <v>99</v>
+      </c>
+      <c r="K8" s="28">
+        <f>SUM(F18:F27)</f>
+        <v>82</v>
+      </c>
+      <c r="L8" s="29">
         <f>SUM(J8:K8)</f>
-        <v>0</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1780,13 +1782,17 @@
         <v>69</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F9" s="11">
+        <v>5</v>
+      </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
@@ -1795,13 +1801,17 @@
         <v>70</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="10">
+        <v>13</v>
+      </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
     </row>
@@ -1810,14 +1820,20 @@
         <v>71</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="11">
+        <v>13</v>
+      </c>
+      <c r="G11" s="11">
+        <v>2</v>
+      </c>
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1830,261 +1846,302 @@
       <c r="D12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="10">
+        <v>13</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="11">
+        <v>8</v>
+      </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
     </row>
     <row r="14" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="10">
+        <v>21</v>
+      </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="11">
+        <v>13</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="10">
+        <v>8</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="2:8" ht="19.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:8" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" s="11">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" s="10">
+        <v>8</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="11">
+        <v>5</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
     <row r="20" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
+      <c r="B20" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="10">
+        <v>13</v>
+      </c>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>106</v>
-      </c>
+      <c r="B21" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="11">
+        <v>8</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="10">
+        <v>8</v>
+      </c>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="11">
+        <v>8</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="10">
+        <v>3</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="16" t="s">
-        <v>98</v>
-      </c>
       <c r="C25" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25" s="11">
+        <v>3</v>
+      </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
-        <v>99</v>
+      <c r="B26" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="10">
+        <v>13</v>
+      </c>
       <c r="G26" s="10"/>
-      <c r="H26" s="15"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="16" t="s">
-        <v>86</v>
+      <c r="B27" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="11">
+        <v>13</v>
+      </c>
       <c r="G27" s="11"/>
-      <c r="H27" s="17"/>
-    </row>
-    <row r="28" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="17"/>
-    </row>
-    <row r="30" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="2:8" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
+      <c r="H27" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B20:H20"/>
+  <mergeCells count="3">
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="J6:L6"/>

</xml_diff>

<commit_message>
Versão atualizada do backlog de Requisitos
</commit_message>
<xml_diff>
--- a/documentos/Backlog Requisitos.xlsx
+++ b/documentos/Backlog Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/henrique_coelho_sptech_school/Documents/SPTECH/Sprint2/sprint2/documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{F7D1B04D-B3ED-4B34-9640-7573DB81BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E07D051-69A4-4F4A-BACB-2288EB9B11AF}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{F7D1B04D-B3ED-4B34-9640-7573DB81BA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0153686B-BB35-4CE3-AE9F-E810496EEE83}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
   </bookViews>
@@ -347,9 +347,6 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>Pontuação</t>
-  </si>
-  <si>
     <t xml:space="preserve">Requisitos do Site </t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>Coletar e validar as informações cadastrais e gravar no banco de dados</t>
+  </si>
+  <si>
+    <t>Pontuação Geral</t>
   </si>
 </sst>
 </file>
@@ -740,6 +740,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -774,15 +783,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1247,23 +1247,23 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
@@ -1623,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7DA6DA-76F6-4BBF-B420-7F89428DFE23}">
   <dimension ref="B2:L27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1639,35 +1639,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
     </row>
     <row r="4" spans="2:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" spans="2:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -1703,18 +1703,18 @@
         <v>5</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F6" s="10">
         <v>13</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
-      <c r="J6" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="K6" s="25"/>
-      <c r="L6" s="26"/>
+      <c r="J6" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="29"/>
     </row>
     <row r="7" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
@@ -1727,7 +1727,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F7" s="11">
         <v>3</v>
@@ -1740,10 +1740,10 @@
         <v>64</v>
       </c>
       <c r="K7" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1757,24 +1757,24 @@
         <v>5</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8" s="10">
         <v>5</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
-      <c r="J8" s="27">
-        <f>SUM(F8:F16)</f>
-        <v>99</v>
-      </c>
-      <c r="K8" s="28">
+      <c r="J8" s="15">
+        <f>SUM(F6:F16)</f>
+        <v>115</v>
+      </c>
+      <c r="K8" s="16">
         <f>SUM(F18:F27)</f>
         <v>82</v>
       </c>
-      <c r="L8" s="29">
-        <f>SUM(J8:K8)</f>
-        <v>181</v>
+      <c r="L8" s="17">
+        <f>SUM(F6:F27)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1788,7 +1788,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F9" s="11">
         <v>5</v>
@@ -1807,7 +1807,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F10" s="10">
         <v>13</v>
@@ -1826,7 +1826,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F11" s="11">
         <v>13</v>
@@ -1847,7 +1847,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="10">
         <v>13</v>
@@ -1866,7 +1866,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F13" s="11">
         <v>8</v>
@@ -1885,7 +1885,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F14" s="10">
         <v>21</v>
@@ -1895,16 +1895,16 @@
     </row>
     <row r="15" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="D15" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F15" s="11">
         <v>13</v>
@@ -1914,16 +1914,16 @@
     </row>
     <row r="16" spans="2:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>115</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>57</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F16" s="10">
         <v>8</v>
@@ -1942,7 +1942,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" s="11">
         <v>3</v>
@@ -1961,7 +1961,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18" s="10">
         <v>8</v>
@@ -1980,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F19" s="11">
         <v>5</v>
@@ -1999,7 +1999,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F20" s="10">
         <v>13</v>
@@ -2018,7 +2018,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21" s="11">
         <v>8</v>
@@ -2037,7 +2037,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F22" s="10">
         <v>8</v>
@@ -2056,7 +2056,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F23" s="11">
         <v>8</v>
@@ -2075,7 +2075,7 @@
         <v>90</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F24" s="10">
         <v>3</v>
@@ -2094,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F25" s="11">
         <v>3</v>
@@ -2113,7 +2113,7 @@
         <v>57</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" s="10">
         <v>13</v>
@@ -2123,16 +2123,16 @@
     </row>
     <row r="27" spans="2:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="D27" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F27" s="11">
         <v>13</v>

</xml_diff>

<commit_message>
Detalhamento das descrições dos requisitos
</commit_message>
<xml_diff>
--- a/documentos/Backlog Requisitos.xlsx
+++ b/documentos/Backlog Requisitos.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/bruno_lima_sptech_school/Documents/git/sprint2/documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Trabalhos\SPTech\1 semestre\PI\repos\sprint2\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="479" documentId="13_ncr:1_{454CC55A-C795-4187-9620-8411508DDD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77D6D20F-D905-414C-B483-BAC9C590BDB1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC87B620-E700-46C5-93BC-051419285E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="OLE_LINK1" localSheetId="1">'Sprint 2'!$C$6</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="170">
   <si>
     <t>Vaga Fácil</t>
   </si>
@@ -261,30 +264,18 @@
     <t>Nome e logo</t>
   </si>
   <si>
-    <t>Criar um nome e uma logo para a nossa empresa</t>
-  </si>
-  <si>
     <t>PP</t>
   </si>
   <si>
-    <t>Configurar os arquivos do projeto na plataforma GitHub para consulta de ambos os integrantes do projeto</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>Configurar a plataforma Trello com todos os requisitos listados neste documento</t>
-  </si>
-  <si>
     <t>Modelagem do Banco de Dados</t>
   </si>
   <si>
     <t>Criação do código Arduino</t>
   </si>
   <si>
-    <t>Criar um código onde será feita a captura de dados do sensor de bloqueio e inclui-los em um gráfico</t>
-  </si>
-  <si>
     <t>GG</t>
   </si>
   <si>
@@ -300,78 +291,33 @@
     <t>Planilha de Riscos do projeto</t>
   </si>
   <si>
-    <t>Criar planilha que irá mostrar quais são os riscos do projeto</t>
-  </si>
-  <si>
-    <t>Especificar quais são os métodos utilizados e suas métricas</t>
-  </si>
-  <si>
-    <t>Criar o protótipo do site institucional das sessões: Início, Sobre Nós, Simulador, Cadastro</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sessão Calculadora </t>
   </si>
   <si>
-    <t>Realizar um cálculo de redução de gastos com base nas informações do cliente</t>
-  </si>
-  <si>
-    <t>Desenvolvimento da lógica e do código da calculadora</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sessão Login </t>
   </si>
   <si>
-    <t xml:space="preserve">Realizar o login do cliente através de um email e uma senha </t>
-  </si>
-  <si>
-    <t>Validação dos dados inseridos pelo usuário e retornar permissão.</t>
-  </si>
-  <si>
     <t>Importante</t>
   </si>
   <si>
     <t xml:space="preserve">Sessão Recuperação de senha </t>
   </si>
   <si>
-    <t>Recuperar uma senha esquecida</t>
-  </si>
-  <si>
-    <t>Recuperar a senha através do envio de um código e a criação de uma nova senha</t>
-  </si>
-  <si>
     <t>Sessão Dashboard</t>
   </si>
   <si>
-    <t>Local que irá aparecer os dados para o usuário em formato de gráfico</t>
-  </si>
-  <si>
     <t xml:space="preserve">Essencial </t>
   </si>
   <si>
     <t xml:space="preserve">G </t>
   </si>
   <si>
-    <t>Conjunto de sessões localizada na parte superior do site</t>
-  </si>
-  <si>
-    <t>Informações sobre cada sessão do site institucional</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sessão Sobre Nós </t>
   </si>
   <si>
-    <t>Informações detalhadas sobre a empresa e a equipe envolvida no projeto</t>
-  </si>
-  <si>
-    <t>Serviços de atendimento ao cliente</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sessão Cadastro </t>
   </si>
   <si>
-    <t xml:space="preserve">Coletar informações do nosso cliente </t>
-  </si>
-  <si>
     <t>Coletar e validar as informações cadastrais e gravar no banco de dados</t>
   </si>
   <si>
@@ -408,12 +354,6 @@
     <t>Responsividade do Site Dashboard</t>
   </si>
   <si>
-    <t>Criar um script com os valores de cada coluna no Banco de Dados local</t>
-  </si>
-  <si>
-    <t>Adaptação das telas para diversos tamanhos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validação e lógica Calculadora </t>
   </si>
   <si>
@@ -444,27 +384,9 @@
     <t>Validação e lógica Perfil</t>
   </si>
   <si>
-    <t>Consultar informações sobre o usuário logado</t>
-  </si>
-  <si>
     <t>Desejável</t>
   </si>
   <si>
-    <t>Confirmar se o sistema está exibir somente a informação do usuário logado</t>
-  </si>
-  <si>
-    <t>Consultar usuários que a pessoa cadastrou e é superior</t>
-  </si>
-  <si>
-    <t>Exibir somente os usuários criados pela pessoa logada</t>
-  </si>
-  <si>
-    <t>Adicionar um usuário no qual a pessoa é superior</t>
-  </si>
-  <si>
-    <t>Verificar e validar se os dados do novo usuário estão corretos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validação e lógica Recuperação de senha </t>
   </si>
   <si>
@@ -501,34 +423,133 @@
     <t>Validação e lógica Expandir</t>
   </si>
   <si>
-    <t>Menu para mudar de sessões no site do dashboard</t>
-  </si>
-  <si>
     <t>Sprint 2.5</t>
   </si>
   <si>
     <t>Fibonacci</t>
   </si>
   <si>
-    <t>Criar um banco de dados na ferramenta MySQL para armazenar informações do cliente e dos sensores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">criar uma estrutura de informações que serve de modelo para o comportamento de um banco de dados </t>
-  </si>
-  <si>
-    <t>Tratar os dados coletados e convertê-los em um gráfico</t>
-  </si>
-  <si>
     <t>Diagrama de Solução (arquitetura técnica do projeto)</t>
   </si>
   <si>
-    <t>Criar uma sequência visual que demonstra a arquitetura técnica do projeto</t>
-  </si>
-  <si>
     <t>Especificação do Analytics/Métricas</t>
   </si>
   <si>
     <t>Criar um diagrama de visão de negócio sobre os nossos serviços ao cliente</t>
+  </si>
+  <si>
+    <t>Criação um nome e uma logo para o projeto.</t>
+  </si>
+  <si>
+    <t>Configurar os arquivos do projeto na plataforma GitHub para consulta dos integrantes do projeto e controle de versionamento.</t>
+  </si>
+  <si>
+    <t>Configurar a plataforma Trello com todos os requisitos listados neste documento.</t>
+  </si>
+  <si>
+    <t>Especificar quais são as métricas empregadas para análise dos dados captados.</t>
+  </si>
+  <si>
+    <t>Criar uma sequência visual que demonstra a arquitetura técnica do projeto.</t>
+  </si>
+  <si>
+    <t>Criar planilha que irá mostrar quais são os riscos do projeto, e medidas empregadas para minimizá-los.</t>
+  </si>
+  <si>
+    <t>Tela do Dashboard onde serão apresentadas todas as unidades cadastradas para o cliente atual. Exibição de tela de informações quando o usuário selecionar uma delas.</t>
+  </si>
+  <si>
+    <t>Informações detalhadas sobre a empresa Vaga Fácil e a equipe envolvida no projeto. Exibição de Missão, Visão e Valores da empresa.</t>
+  </si>
+  <si>
+    <t>Tela contendo Informações resumidas sobre cada sessão do site institucional.</t>
+  </si>
+  <si>
+    <t>Tela para realização do login do cliente através de um e-mail e uma senha. Links para Recuperação de Senha e Tela de Cadastro.</t>
+  </si>
+  <si>
+    <t>Consultar usuários que a pessoa cadastrou, e é superior aos mesmos. Presença de opção para excluir usuários.</t>
+  </si>
+  <si>
+    <t>Validação dos dados inseridos pelo usuário e inserção dos mesmos no Banco de Dados</t>
+  </si>
+  <si>
+    <t>Confirmar se há um usuário logado, e exibir somente as informações do mesmo.</t>
+  </si>
+  <si>
+    <t>Recuperar a senha através do envio de um código ao e-mail inserido pelo usuário, e validação e inserção de nova senha.</t>
+  </si>
+  <si>
+    <t>Receber dados do banco para exibir somente os usuários criados pela pessoa logada.</t>
+  </si>
+  <si>
+    <t>Criar um banco de dados na ferramenta MySQL para armazenar informações dos clientes e dos sensores.</t>
+  </si>
+  <si>
+    <t>Criação de código que será inserido no Arduino, onde será feita a captura de dados do sensor e envio dos mesmos através de porta serial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar uma estrutura de informações que serve de modelo para o comportamento de um banco de dados </t>
+  </si>
+  <si>
+    <t>Criar o protótipo do site institucional das sessões: Início, Sobre Nós, Simulador, Login, Recuperação de senha, Dashboard e Cadastro.</t>
+  </si>
+  <si>
+    <t>Adaptação das telas para diversos tamanhos.</t>
+  </si>
+  <si>
+    <t>Obter dados do banco de dados para as filiais da empresa do cliente. Atribuição dos dados aos gráficos e KPIs construídos em ChartJS.</t>
+  </si>
+  <si>
+    <t>Desenvolvimento da lógica e do código da calculadora. Recuperar informações dos bairros inseridos pelo cliente e aplica-los ao lucro.</t>
+  </si>
+  <si>
+    <t>Tratar os dados provenientes do Banco de Dados e convertê-los em gráficos e KPIs.</t>
+  </si>
+  <si>
+    <t> Obter dados do banco de dados, contendo informações dos bairros e suas respectivas populações. Obter informações das ruas e seus respectivos sensores.</t>
+  </si>
+  <si>
+    <t>Script com as definições de Banco de Dados e Tabelas para funcionamento do sistema. Inserção de valores iniciais.</t>
+  </si>
+  <si>
+    <t>Criação de API NodeJS para receber os dados vindos do Arduino e então cadastrá-los no Banco de Dados.</t>
+  </si>
+  <si>
+    <t>Conjunto de atalhos localizada na parte superior do site. Contendo: Logo; Início; Sobre Nós; Calculadora; Fale Conosco; Login, para acesso ao Dashboard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodapé contendo 3 sessôes: Logo; Links (mesmos links presentes no cabeçalho); Links para mídias sociais. </t>
+  </si>
+  <si>
+    <t>Tela para processo de recuperação de senha, contendo 3 etapas: Solicitação de email da conta; Input de código enviado ao email; Input de nova senha, em duplicata.</t>
+  </si>
+  <si>
+    <t>Menu para mudar de sessões no site do dashboard, contendo seguintes links: Dashboard; Acompanhar; Expandir; Perfil; Lista de usuários; Adicionar usuário; Site Institucional.</t>
+  </si>
+  <si>
+    <t>Tela para superiores adicionarem funcionários, para que os mesmos possam utilizar o sistema. Contendo campos: Nome; Sobrenome; Data de Nascimento; CPF; Telefone; E-mail; Senha (em duplicata).</t>
+  </si>
+  <si>
+    <t>Tela do Dashboard onde o usuário poderá buscar por novos locais para expandir o negócio. Dividido em três Telas: Tela para selecionar bairro (Zona de São Paulo; Faixa etária da população; Faixa de renda da população); Tela para selecionar rua (Faixa etária da população; Faixa de renda da população); Tela mostrando informações da rua (Tipo de dia (dia da semana, fim de semana, feriado); Dia da semana; Mês; Vaga específica).</t>
+  </si>
+  <si>
+    <t>Tela para consulta de informações sobre o usuário logado: Nome; Data de Nascimento; CPF Telefone; E-mail; Nome da Empresa; CEP e Endereço da Empresa; CNPJ da Empresa; Setor, Área e Cargo de atuação; Jornada de Trabalho. Conterá tela para alteração de nome e imagem de perfil.</t>
+  </si>
+  <si>
+    <t>Verificar e validar se os dados do novo usuário estão corretos. Validação de: Data de Nascimento; CPF; Telefone; E-mail; Senha.</t>
+  </si>
+  <si>
+    <t>Página de serviços de atendimento ao cliente, contendo informações de contato e formulário para envio de mensagens, solicitando: Nome; E-mail; Telefone; Mensagem.</t>
+  </si>
+  <si>
+    <t>Coletar informações do cliente para cadastro no Banco de Dados: Nome; Sobrenome; Data de Nascimento; CPF; Telefone; Razão Social da Empresa; CNPJ da Empresa; CEP da Empresa; Número da Empresa; Complemento da Empresa; E-mail; Senha (em duplicata).</t>
+  </si>
+  <si>
+    <t>Tela para clientes simularem possíveis ganhos que podem ter através da utilização de nossa ferramenta. Sessão informativa explicando o cálculo e campos de: Lucro atual; Bairro atual; Bairro novo. Sistema então retorna um novo lucro com base nestas informações.</t>
+  </si>
+  <si>
+    <t>Tela que irá exibir os dados para o usuário em forma de gráficos e KPIs. Filtros: Endereço; Tipo de dia (dia de semana, fim de semana, feriado); Dia da semana; Mês; Vaga específica.</t>
   </si>
 </sst>
 </file>
@@ -993,7 +1014,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2039,7 +2060,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2726,8 +2747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16856E6-9DCD-40AD-91F7-EC610FDB522F}">
   <dimension ref="A2:O56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,7 +2810,7 @@
         <v>66</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>67</v>
@@ -2801,16 +2822,16 @@
     <row r="6" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="10" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>104</v>
+        <v>158</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" s="10">
         <v>3</v>
@@ -2825,19 +2846,19 @@
         <v>72</v>
       </c>
       <c r="K6" s="17" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2846,13 +2867,13 @@
         <v>73</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>75</v>
       </c>
       <c r="F7" s="11">
         <v>3</v>
@@ -2886,16 +2907,16 @@
     <row r="8" spans="1:15" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="10" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>110</v>
+        <v>159</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="10">
         <v>3</v>
@@ -2910,16 +2931,16 @@
     <row r="9" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="11">
         <v>3</v>
@@ -2931,37 +2952,37 @@
         <v>2</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="O9" s="17" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="10" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10" s="10">
         <v>5</v>
@@ -3000,16 +3021,16 @@
     <row r="11" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="11" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11" s="11">
         <v>5</v>
@@ -3025,16 +3046,16 @@
     <row r="12" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="10" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F12" s="10">
         <v>5</v>
@@ -3049,16 +3070,16 @@
     <row r="13" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="11" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F13" s="11">
         <v>5</v>
@@ -3073,16 +3094,16 @@
     <row r="14" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="10" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F14" s="10">
         <v>5</v>
@@ -3097,16 +3118,16 @@
     <row r="15" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15" s="11">
         <v>5</v>
@@ -3121,14 +3142,16 @@
     <row r="16" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="10"/>
+        <v>123</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>138</v>
+      </c>
       <c r="D16" s="10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F16" s="10">
         <v>5</v>
@@ -3140,19 +3163,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="11" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17" s="11">
         <v>5</v>
@@ -3164,17 +3187,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="10"/>
+        <v>125</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>163</v>
+      </c>
       <c r="D18" s="10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" s="10">
         <v>5</v>
@@ -3186,19 +3211,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
       <c r="B19" s="11" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F19" s="11">
         <v>5</v>
@@ -3213,16 +3238,16 @@
     <row r="20" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
       <c r="B20" s="10" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F20" s="10">
         <v>5</v>
@@ -3237,16 +3262,16 @@
     <row r="21" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="11" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F21" s="11">
         <v>5</v>
@@ -3261,16 +3286,16 @@
     <row r="22" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
       <c r="B22" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F22" s="10">
         <v>8</v>
@@ -3285,16 +3310,16 @@
     <row r="23" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
       <c r="B23" s="11" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F23" s="11">
         <v>8</v>
@@ -3310,16 +3335,16 @@
     <row r="24" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="10" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F24" s="10">
         <v>8</v>
@@ -3334,16 +3359,16 @@
     <row r="25" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="11" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F25" s="11">
         <v>8</v>
@@ -3358,16 +3383,16 @@
     <row r="26" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="10" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F26" s="10">
         <v>8</v>
@@ -3382,16 +3407,16 @@
     <row r="27" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="D27" s="11" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F27" s="11">
         <v>8</v>
@@ -3406,16 +3431,16 @@
     <row r="28" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="10" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F28" s="10">
         <v>8</v>
@@ -3430,16 +3455,16 @@
     <row r="29" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="11" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F29" s="11">
         <v>8</v>
@@ -3454,16 +3479,16 @@
     <row r="30" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
       <c r="B30" s="10" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F30" s="10">
         <v>8</v>
@@ -3478,10 +3503,10 @@
     <row r="31" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="11" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>7</v>
@@ -3502,10 +3527,10 @@
     <row r="32" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>7</v>
@@ -3550,10 +3575,10 @@
     <row r="34" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>7</v>
@@ -3574,10 +3599,10 @@
     <row r="35" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="11" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>7</v>
@@ -3598,10 +3623,10 @@
     <row r="36" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="10" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>59</v>
@@ -3622,10 +3647,10 @@
     <row r="37" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="11" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>59</v>
@@ -3643,13 +3668,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="10" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>110</v>
+        <v>167</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>7</v>
@@ -3667,13 +3692,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>91</v>
+        <v>168</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>7</v>
@@ -3694,16 +3719,16 @@
     <row r="40" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="10" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F40" s="10">
         <v>13</v>
@@ -3718,11 +3743,13 @@
     <row r="41" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C41" s="11"/>
+        <v>124</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>152</v>
+      </c>
       <c r="D41" s="11" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>71</v>
@@ -3740,10 +3767,10 @@
     <row r="42" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="10" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>7</v>
@@ -3764,10 +3791,10 @@
     <row r="43" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="11" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>7</v>
@@ -3788,16 +3815,16 @@
     <row r="44" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="10" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F44" s="10">
         <v>13</v>
@@ -3812,11 +3839,13 @@
     <row r="45" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C45" s="11"/>
+        <v>126</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="D45" s="11" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>71</v>
@@ -3834,16 +3863,16 @@
     <row r="46" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="10" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F46" s="10">
         <v>21</v>
@@ -3861,13 +3890,13 @@
         <v>8</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>9</v>
+        <v>157</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F47" s="11">
         <v>21</v>

</xml_diff>